<commit_message>
Changed lose to loss
</commit_message>
<xml_diff>
--- a/AgentToTrain.xlsx
+++ b/AgentToTrain.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ConnectFourRL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA2BFE5-E134-4D8C-93E1-F5BD17F21416}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F9B916-A540-4C1F-A904-133A231FB56C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2E35238C-8557-40CC-9A92-1D08C6546023}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>RewardDecay</t>
   </si>
   <si>
-    <t>Agent</t>
-  </si>
-  <si>
     <t>MinMax</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>BasicBitchV1</t>
+  </si>
+  <si>
+    <t>AgentSize</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,10 +541,10 @@
         <v>12</v>
       </c>
       <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
         <v>13</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
       </c>
       <c r="O1" t="s">
         <v>0</v>
@@ -552,7 +552,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -582,21 +582,21 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L2">
         <v>0.99</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -626,21 +626,21 @@
         <v>0.1</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L3">
         <v>0.99</v>
       </c>
       <c r="M3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>50</v>
@@ -670,21 +670,21 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L4">
         <v>0.99</v>
       </c>
       <c r="M4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>500</v>
@@ -714,21 +714,21 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L5">
         <v>0.85</v>
       </c>
       <c r="M5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" t="s">
         <v>25</v>
-      </c>
-      <c r="N5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>500</v>
@@ -758,21 +758,21 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L6">
         <v>0.99</v>
       </c>
       <c r="M6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" t="s">
         <v>25</v>
-      </c>
-      <c r="N6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>500</v>
@@ -802,21 +802,21 @@
         <v>0.05</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L7">
         <v>0.9</v>
       </c>
       <c r="M7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>200</v>
@@ -846,21 +846,21 @@
         <v>0.1</v>
       </c>
       <c r="K8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L8">
         <v>0.4</v>
       </c>
       <c r="M8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>200</v>
@@ -890,21 +890,21 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L9">
         <v>0.4</v>
       </c>
       <c r="M9" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" t="s">
         <v>25</v>
-      </c>
-      <c r="N9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>200</v>
@@ -934,21 +934,21 @@
         <v>0.1</v>
       </c>
       <c r="K10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L10">
         <v>0.9</v>
       </c>
       <c r="M10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>100</v>
@@ -978,21 +978,21 @@
         <v>0.1</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L11">
         <v>0.99</v>
       </c>
       <c r="M11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>100</v>
@@ -1022,16 +1022,16 @@
         <v>0.1</v>
       </c>
       <c r="K12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L12">
         <v>0.99</v>
       </c>
       <c r="M12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First run done in xlsx before stop
</commit_message>
<xml_diff>
--- a/AgentToTrain.xlsx
+++ b/AgentToTrain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ConnectFourRL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F9B916-A540-4C1F-A904-133A231FB56C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0E202C-F6FB-4FA7-B9CB-A423696F7625}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2E35238C-8557-40CC-9A92-1D08C6546023}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2E35238C-8557-40CC-9A92-1D08C6546023}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>Neptune</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>AgentSize</t>
+  </si>
+  <si>
+    <t>CON-81</t>
   </si>
 </sst>
 </file>
@@ -485,7 +488,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,6 +596,9 @@
       <c r="N2" t="s">
         <v>26</v>
       </c>
+      <c r="O2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>